<commit_message>
Fixed tissue numbering in exercise spreadsheets
</commit_message>
<xml_diff>
--- a/Session 2/Exercises/AmD_Training_P01.xlsx
+++ b/Session 2/Exercises/AmD_Training_P01.xlsx
@@ -103,1759 +103,1759 @@
     <t>A01</t>
   </si>
   <si>
+    <t>AmD_Tissue_1</t>
+  </si>
+  <si>
+    <t>USNM:Birds:647764</t>
+  </si>
+  <si>
+    <t>USNM</t>
+  </si>
+  <si>
+    <t>Birds</t>
+  </si>
+  <si>
+    <t>647764</t>
+  </si>
+  <si>
+    <t>Threskiornis aethiopicus</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Camp Lemonnier, ca 5.5 km SE Djibouti</t>
+  </si>
+  <si>
+    <t>11.5417</t>
+  </si>
+  <si>
+    <t>43.1667</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>W. Beveridge</t>
+  </si>
+  <si>
+    <t>Animalia</t>
+  </si>
+  <si>
+    <t>Chordata</t>
+  </si>
+  <si>
+    <t>Aves</t>
+  </si>
+  <si>
+    <t>Ciconiiformes</t>
+  </si>
+  <si>
+    <t>Threskiornithidae</t>
+  </si>
+  <si>
+    <t>Threskiornis</t>
+  </si>
+  <si>
+    <t>aethiopicus</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
     <t>AmD_Tissue_2</t>
   </si>
   <si>
-    <t>USNM:Birds:647764</t>
-  </si>
-  <si>
-    <t>USNM</t>
-  </si>
-  <si>
-    <t>Birds</t>
-  </si>
-  <si>
-    <t>647764</t>
-  </si>
-  <si>
-    <t>Threskiornis aethiopicus</t>
-  </si>
-  <si>
-    <t>Djibouti</t>
-  </si>
-  <si>
-    <t>Camp Lemonnier, ca 5.5 km SE Djibouti</t>
-  </si>
-  <si>
-    <t>11.5417</t>
-  </si>
-  <si>
-    <t>43.1667</t>
-  </si>
-  <si>
-    <t>2014</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>W. Beveridge</t>
-  </si>
-  <si>
-    <t>Animalia</t>
-  </si>
-  <si>
-    <t>Chordata</t>
-  </si>
-  <si>
-    <t>Aves</t>
-  </si>
-  <si>
-    <t>Ciconiiformes</t>
-  </si>
-  <si>
-    <t>Threskiornithidae</t>
-  </si>
-  <si>
-    <t>Threskiornis</t>
-  </si>
-  <si>
-    <t>aethiopicus</t>
-  </si>
-  <si>
-    <t>B01</t>
+    <t>USNM:Birds:647765</t>
+  </si>
+  <si>
+    <t>647765</t>
+  </si>
+  <si>
+    <t>Corvus splendens</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>S. Peurach</t>
+  </si>
+  <si>
+    <t>Passeriformes</t>
+  </si>
+  <si>
+    <t>Corvidae</t>
+  </si>
+  <si>
+    <t>Corvus</t>
+  </si>
+  <si>
+    <t>splendens</t>
+  </si>
+  <si>
+    <t>C01</t>
   </si>
   <si>
     <t>AmD_Tissue_3</t>
   </si>
   <si>
-    <t>USNM:Birds:647765</t>
-  </si>
-  <si>
-    <t>647765</t>
-  </si>
-  <si>
-    <t>Corvus splendens</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>S. Peurach</t>
-  </si>
-  <si>
-    <t>Passeriformes</t>
-  </si>
-  <si>
-    <t>Corvidae</t>
-  </si>
-  <si>
-    <t>Corvus</t>
-  </si>
-  <si>
-    <t>splendens</t>
-  </si>
-  <si>
-    <t>C01</t>
+    <t>USNM:Birds:647766</t>
+  </si>
+  <si>
+    <t>647766</t>
+  </si>
+  <si>
+    <t>D01</t>
   </si>
   <si>
     <t>AmD_Tissue_4</t>
   </si>
   <si>
-    <t>USNM:Birds:647766</t>
-  </si>
-  <si>
-    <t>647766</t>
-  </si>
-  <si>
-    <t>D01</t>
+    <t>USNM:Birds:647762</t>
+  </si>
+  <si>
+    <t>647762</t>
+  </si>
+  <si>
+    <t>Dromas ardeola</t>
+  </si>
+  <si>
+    <t>Charadriiformes</t>
+  </si>
+  <si>
+    <t>Dromadidae</t>
+  </si>
+  <si>
+    <t>Dromas</t>
+  </si>
+  <si>
+    <t>ardeola</t>
+  </si>
+  <si>
+    <t>E01</t>
   </si>
   <si>
     <t>AmD_Tissue_5</t>
   </si>
   <si>
-    <t>USNM:Birds:647762</t>
-  </si>
-  <si>
-    <t>647762</t>
-  </si>
-  <si>
-    <t>Dromas ardeola</t>
-  </si>
-  <si>
-    <t>Charadriiformes</t>
-  </si>
-  <si>
-    <t>Dromadidae</t>
-  </si>
-  <si>
-    <t>Dromas</t>
-  </si>
-  <si>
-    <t>ardeola</t>
-  </si>
-  <si>
-    <t>E01</t>
+    <t>USNM:Birds:647767</t>
+  </si>
+  <si>
+    <t>647767</t>
+  </si>
+  <si>
+    <t>M. Klope</t>
+  </si>
+  <si>
+    <t>F01</t>
   </si>
   <si>
     <t>AmD_Tissue_6</t>
   </si>
   <si>
-    <t>USNM:Birds:647767</t>
-  </si>
-  <si>
-    <t>647767</t>
-  </si>
-  <si>
-    <t>M. Klope</t>
-  </si>
-  <si>
-    <t>F01</t>
+    <t>USNM:Birds:647768</t>
+  </si>
+  <si>
+    <t>647768</t>
+  </si>
+  <si>
+    <t>Egretta gularis</t>
+  </si>
+  <si>
+    <t>Ardeidae</t>
+  </si>
+  <si>
+    <t>Egretta</t>
+  </si>
+  <si>
+    <t>gularis</t>
+  </si>
+  <si>
+    <t>G01</t>
   </si>
   <si>
     <t>AmD_Tissue_7</t>
   </si>
   <si>
-    <t>USNM:Birds:647768</t>
-  </si>
-  <si>
-    <t>647768</t>
-  </si>
-  <si>
-    <t>Egretta gularis</t>
-  </si>
-  <si>
-    <t>Ardeidae</t>
-  </si>
-  <si>
-    <t>Egretta</t>
-  </si>
-  <si>
-    <t>gularis</t>
-  </si>
-  <si>
-    <t>G01</t>
+    <t>USNM:Birds:647769</t>
+  </si>
+  <si>
+    <t>647769</t>
+  </si>
+  <si>
+    <t>Calidris ferruginea</t>
+  </si>
+  <si>
+    <t>Scolopacidae</t>
+  </si>
+  <si>
+    <t>Calidris</t>
+  </si>
+  <si>
+    <t>ferruginea</t>
+  </si>
+  <si>
+    <t>H01</t>
   </si>
   <si>
     <t>AmD_Tissue_8</t>
   </si>
   <si>
-    <t>USNM:Birds:647769</t>
-  </si>
-  <si>
-    <t>647769</t>
-  </si>
-  <si>
-    <t>Calidris ferruginea</t>
-  </si>
-  <si>
-    <t>Scolopacidae</t>
-  </si>
-  <si>
-    <t>Calidris</t>
-  </si>
-  <si>
-    <t>ferruginea</t>
-  </si>
-  <si>
-    <t>H01</t>
+    <t>USNM:Birds:647770</t>
+  </si>
+  <si>
+    <t>647770</t>
+  </si>
+  <si>
+    <t>Hirundo rustica</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Hirundinidae</t>
+  </si>
+  <si>
+    <t>Hirundo</t>
+  </si>
+  <si>
+    <t>rustica</t>
+  </si>
+  <si>
+    <t>A02</t>
   </si>
   <si>
     <t>AmD_Tissue_9</t>
   </si>
   <si>
-    <t>USNM:Birds:647770</t>
-  </si>
-  <si>
-    <t>647770</t>
-  </si>
-  <si>
-    <t>Hirundo rustica</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Hirundinidae</t>
-  </si>
-  <si>
-    <t>Hirundo</t>
-  </si>
-  <si>
-    <t>rustica</t>
-  </si>
-  <si>
-    <t>A02</t>
+    <t>USNM:Birds:647771</t>
+  </si>
+  <si>
+    <t>647771</t>
+  </si>
+  <si>
+    <t>Passer castanopterus</t>
+  </si>
+  <si>
+    <t>Ploceidae</t>
+  </si>
+  <si>
+    <t>Passer</t>
+  </si>
+  <si>
+    <t>castanopterus</t>
+  </si>
+  <si>
+    <t>B02</t>
   </si>
   <si>
     <t>AmD_Tissue_10</t>
   </si>
   <si>
-    <t>USNM:Birds:647771</t>
-  </si>
-  <si>
-    <t>647771</t>
-  </si>
-  <si>
-    <t>Passer castanopterus</t>
-  </si>
-  <si>
-    <t>Ploceidae</t>
-  </si>
-  <si>
-    <t>Passer</t>
-  </si>
-  <si>
-    <t>castanopterus</t>
-  </si>
-  <si>
-    <t>B02</t>
+    <t>USNM:Birds:647772</t>
+  </si>
+  <si>
+    <t>647772</t>
+  </si>
+  <si>
+    <t>C02</t>
   </si>
   <si>
     <t>AmD_Tissue_11</t>
   </si>
   <si>
-    <t>USNM:Birds:647772</t>
-  </si>
-  <si>
-    <t>647772</t>
-  </si>
-  <si>
-    <t>C02</t>
+    <t>USNM:Birds:647773</t>
+  </si>
+  <si>
+    <t>647773</t>
+  </si>
+  <si>
+    <t>Lagonosticta senegala</t>
+  </si>
+  <si>
+    <t>Estrildidae</t>
+  </si>
+  <si>
+    <t>Lagonosticta</t>
+  </si>
+  <si>
+    <t>senegala</t>
+  </si>
+  <si>
+    <t>D02</t>
   </si>
   <si>
     <t>AmD_Tissue_12</t>
   </si>
   <si>
-    <t>USNM:Birds:647773</t>
-  </si>
-  <si>
-    <t>647773</t>
-  </si>
-  <si>
-    <t>Lagonosticta senegala</t>
-  </si>
-  <si>
-    <t>Estrildidae</t>
-  </si>
-  <si>
-    <t>Lagonosticta</t>
-  </si>
-  <si>
-    <t>senegala</t>
-  </si>
-  <si>
-    <t>D02</t>
+    <t>USNM:Birds:647774</t>
+  </si>
+  <si>
+    <t>647774</t>
+  </si>
+  <si>
+    <t>Calidris minuta</t>
+  </si>
+  <si>
+    <t>minuta</t>
+  </si>
+  <si>
+    <t>E02</t>
   </si>
   <si>
     <t>AmD_Tissue_13</t>
   </si>
   <si>
-    <t>USNM:Birds:647774</t>
-  </si>
-  <si>
-    <t>647774</t>
-  </si>
-  <si>
-    <t>Calidris minuta</t>
-  </si>
-  <si>
-    <t>minuta</t>
-  </si>
-  <si>
-    <t>E02</t>
+    <t>USNM:Birds:647775</t>
+  </si>
+  <si>
+    <t>647775</t>
+  </si>
+  <si>
+    <t>Muscicapa striata</t>
+  </si>
+  <si>
+    <t>Muscicapidae</t>
+  </si>
+  <si>
+    <t>Muscicapa</t>
+  </si>
+  <si>
+    <t>striata</t>
+  </si>
+  <si>
+    <t>F02</t>
   </si>
   <si>
     <t>AmD_Tissue_14</t>
   </si>
   <si>
-    <t>USNM:Birds:647775</t>
-  </si>
-  <si>
-    <t>647775</t>
-  </si>
-  <si>
-    <t>Muscicapa striata</t>
-  </si>
-  <si>
-    <t>Muscicapidae</t>
-  </si>
-  <si>
-    <t>Muscicapa</t>
-  </si>
-  <si>
-    <t>striata</t>
-  </si>
-  <si>
-    <t>F02</t>
+    <t>USNM:Birds:647776</t>
+  </si>
+  <si>
+    <t>647776</t>
+  </si>
+  <si>
+    <t>Streptopelia roseogrisea</t>
+  </si>
+  <si>
+    <t>Columbiformes</t>
+  </si>
+  <si>
+    <t>Columbidae</t>
+  </si>
+  <si>
+    <t>Streptopelia</t>
+  </si>
+  <si>
+    <t>roseogrisea</t>
+  </si>
+  <si>
+    <t>G02</t>
   </si>
   <si>
     <t>AmD_Tissue_15</t>
   </si>
   <si>
-    <t>USNM:Birds:647776</t>
-  </si>
-  <si>
-    <t>647776</t>
-  </si>
-  <si>
-    <t>Streptopelia roseogrisea</t>
-  </si>
-  <si>
-    <t>Columbiformes</t>
-  </si>
-  <si>
-    <t>Columbidae</t>
-  </si>
-  <si>
-    <t>Streptopelia</t>
-  </si>
-  <si>
-    <t>roseogrisea</t>
-  </si>
-  <si>
-    <t>G02</t>
+    <t>USNM:Birds:647892</t>
+  </si>
+  <si>
+    <t>647892</t>
+  </si>
+  <si>
+    <t>Motacilla alba</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>United States Navy</t>
+  </si>
+  <si>
+    <t>Motacillidae</t>
+  </si>
+  <si>
+    <t>Motacilla</t>
+  </si>
+  <si>
+    <t>alba</t>
+  </si>
+  <si>
+    <t>H02</t>
   </si>
   <si>
     <t>AmD_Tissue_16</t>
   </si>
   <si>
-    <t>USNM:Birds:647892</t>
-  </si>
-  <si>
-    <t>647892</t>
-  </si>
-  <si>
-    <t>Motacilla alba</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>United States Navy</t>
-  </si>
-  <si>
-    <t>Motacillidae</t>
-  </si>
-  <si>
-    <t>Motacilla</t>
-  </si>
-  <si>
-    <t>alba</t>
-  </si>
-  <si>
-    <t>H02</t>
+    <t>USNM:Birds:647778</t>
+  </si>
+  <si>
+    <t>647778</t>
+  </si>
+  <si>
+    <t>Oena capensis</t>
+  </si>
+  <si>
+    <t>Oena</t>
+  </si>
+  <si>
+    <t>capensis</t>
+  </si>
+  <si>
+    <t>A03</t>
   </si>
   <si>
     <t>AmD_Tissue_17</t>
   </si>
   <si>
-    <t>USNM:Birds:647778</t>
-  </si>
-  <si>
-    <t>647778</t>
-  </si>
-  <si>
-    <t>Oena capensis</t>
-  </si>
-  <si>
-    <t>Oena</t>
-  </si>
-  <si>
-    <t>capensis</t>
-  </si>
-  <si>
-    <t>A03</t>
+    <t>USNM:Birds:647779</t>
+  </si>
+  <si>
+    <t>647779</t>
+  </si>
+  <si>
+    <t>Pycnonotus barbatus</t>
+  </si>
+  <si>
+    <t>Pycnonotidae</t>
+  </si>
+  <si>
+    <t>Pycnonotus</t>
+  </si>
+  <si>
+    <t>barbatus</t>
+  </si>
+  <si>
+    <t>B03</t>
   </si>
   <si>
     <t>AmD_Tissue_18</t>
   </si>
   <si>
-    <t>USNM:Birds:647779</t>
-  </si>
-  <si>
-    <t>647779</t>
-  </si>
-  <si>
-    <t>Pycnonotus barbatus</t>
-  </si>
-  <si>
-    <t>Pycnonotidae</t>
-  </si>
-  <si>
-    <t>Pycnonotus</t>
-  </si>
-  <si>
-    <t>barbatus</t>
-  </si>
-  <si>
-    <t>B03</t>
+    <t>USNM:Birds:647780</t>
+  </si>
+  <si>
+    <t>647780</t>
+  </si>
+  <si>
+    <t>Ploceus galbula</t>
+  </si>
+  <si>
+    <t>Ploceus</t>
+  </si>
+  <si>
+    <t>galbula</t>
+  </si>
+  <si>
+    <t>C03</t>
   </si>
   <si>
     <t>AmD_Tissue_19</t>
   </si>
   <si>
-    <t>USNM:Birds:647780</t>
-  </si>
-  <si>
-    <t>647780</t>
-  </si>
-  <si>
-    <t>Ploceus galbula</t>
-  </si>
-  <si>
-    <t>Ploceus</t>
-  </si>
-  <si>
-    <t>galbula</t>
-  </si>
-  <si>
-    <t>C03</t>
+    <t>USNM:Birds:647781</t>
+  </si>
+  <si>
+    <t>647781</t>
+  </si>
+  <si>
+    <t>Merops persicus</t>
+  </si>
+  <si>
+    <t>Coraciiformes</t>
+  </si>
+  <si>
+    <t>Meropidae</t>
+  </si>
+  <si>
+    <t>Merops</t>
+  </si>
+  <si>
+    <t>persicus</t>
+  </si>
+  <si>
+    <t>D03</t>
   </si>
   <si>
     <t>AmD_Tissue_20</t>
   </si>
   <si>
-    <t>USNM:Birds:647781</t>
-  </si>
-  <si>
-    <t>647781</t>
-  </si>
-  <si>
-    <t>Merops persicus</t>
-  </si>
-  <si>
-    <t>Coraciiformes</t>
-  </si>
-  <si>
-    <t>Meropidae</t>
-  </si>
-  <si>
-    <t>Merops</t>
-  </si>
-  <si>
-    <t>persicus</t>
-  </si>
-  <si>
-    <t>D03</t>
+    <t>USNM:Birds:647782</t>
+  </si>
+  <si>
+    <t>647782</t>
+  </si>
+  <si>
+    <t>Erythropygia galactotes</t>
+  </si>
+  <si>
+    <t>Turdidae</t>
+  </si>
+  <si>
+    <t>Erythropygia</t>
+  </si>
+  <si>
+    <t>galactotes</t>
+  </si>
+  <si>
+    <t>E03</t>
   </si>
   <si>
     <t>AmD_Tissue_21</t>
   </si>
   <si>
-    <t>USNM:Birds:647782</t>
-  </si>
-  <si>
-    <t>647782</t>
-  </si>
-  <si>
-    <t>Erythropygia galactotes</t>
-  </si>
-  <si>
-    <t>Turdidae</t>
-  </si>
-  <si>
-    <t>Erythropygia</t>
-  </si>
-  <si>
-    <t>galactotes</t>
-  </si>
-  <si>
-    <t>E03</t>
+    <t>USNM:Birds:647783</t>
+  </si>
+  <si>
+    <t>647783</t>
+  </si>
+  <si>
+    <t>F03</t>
   </si>
   <si>
     <t>AmD_Tissue_22</t>
   </si>
   <si>
-    <t>USNM:Birds:647783</t>
-  </si>
-  <si>
-    <t>647783</t>
-  </si>
-  <si>
-    <t>F03</t>
+    <t>USNM:Birds:647784</t>
+  </si>
+  <si>
+    <t>647784</t>
+  </si>
+  <si>
+    <t>G03</t>
   </si>
   <si>
     <t>AmD_Tissue_23</t>
   </si>
   <si>
-    <t>USNM:Birds:647784</t>
-  </si>
-  <si>
-    <t>647784</t>
-  </si>
-  <si>
-    <t>G03</t>
+    <t>USNM:Birds:647785</t>
+  </si>
+  <si>
+    <t>647785</t>
+  </si>
+  <si>
+    <t>Lanius collurio</t>
+  </si>
+  <si>
+    <t>Laniidae</t>
+  </si>
+  <si>
+    <t>Lanius</t>
+  </si>
+  <si>
+    <t>collurio</t>
+  </si>
+  <si>
+    <t>H03</t>
   </si>
   <si>
     <t>AmD_Tissue_24</t>
   </si>
   <si>
-    <t>USNM:Birds:647785</t>
-  </si>
-  <si>
-    <t>647785</t>
-  </si>
-  <si>
-    <t>Lanius collurio</t>
-  </si>
-  <si>
-    <t>Laniidae</t>
-  </si>
-  <si>
-    <t>Lanius</t>
-  </si>
-  <si>
-    <t>collurio</t>
-  </si>
-  <si>
-    <t>H03</t>
+    <t>USNM:Birds:647786</t>
+  </si>
+  <si>
+    <t>647786</t>
+  </si>
+  <si>
+    <t>A. Alvarez</t>
+  </si>
+  <si>
+    <t>A04</t>
   </si>
   <si>
     <t>AmD_Tissue_25</t>
   </si>
   <si>
-    <t>USNM:Birds:647786</t>
-  </si>
-  <si>
-    <t>647786</t>
-  </si>
-  <si>
-    <t>A. Alvarez</t>
-  </si>
-  <si>
-    <t>A04</t>
+    <t>USNM:Birds:647787</t>
+  </si>
+  <si>
+    <t>647787</t>
+  </si>
+  <si>
+    <t>B04</t>
   </si>
   <si>
     <t>AmD_Tissue_26</t>
   </si>
   <si>
-    <t>USNM:Birds:647787</t>
-  </si>
-  <si>
-    <t>647787</t>
-  </si>
-  <si>
-    <t>B04</t>
+    <t>USNM:Birds:647788</t>
+  </si>
+  <si>
+    <t>647788</t>
+  </si>
+  <si>
+    <t>C04</t>
   </si>
   <si>
     <t>AmD_Tissue_27</t>
   </si>
   <si>
-    <t>USNM:Birds:647788</t>
-  </si>
-  <si>
-    <t>647788</t>
-  </si>
-  <si>
-    <t>C04</t>
+    <t>USNM:Birds:647789</t>
+  </si>
+  <si>
+    <t>647789</t>
+  </si>
+  <si>
+    <t>Nectarinia venusta</t>
+  </si>
+  <si>
+    <t>Nectariniidae</t>
+  </si>
+  <si>
+    <t>Nectarinia</t>
+  </si>
+  <si>
+    <t>venusta</t>
+  </si>
+  <si>
+    <t>D04</t>
   </si>
   <si>
     <t>AmD_Tissue_28</t>
   </si>
   <si>
-    <t>USNM:Birds:647789</t>
-  </si>
-  <si>
-    <t>647789</t>
-  </si>
-  <si>
-    <t>Nectarinia venusta</t>
-  </si>
-  <si>
-    <t>Nectariniidae</t>
-  </si>
-  <si>
-    <t>Nectarinia</t>
-  </si>
-  <si>
-    <t>venusta</t>
-  </si>
-  <si>
-    <t>D04</t>
+    <t>USNM:Birds:647790</t>
+  </si>
+  <si>
+    <t>647790</t>
+  </si>
+  <si>
+    <t>E04</t>
   </si>
   <si>
     <t>AmD_Tissue_29</t>
   </si>
   <si>
-    <t>USNM:Birds:647790</t>
-  </si>
-  <si>
-    <t>647790</t>
-  </si>
-  <si>
-    <t>E04</t>
+    <t>USNM:Birds:647791</t>
+  </si>
+  <si>
+    <t>647791</t>
+  </si>
+  <si>
+    <t>F04</t>
   </si>
   <si>
     <t>AmD_Tissue_30</t>
   </si>
   <si>
-    <t>USNM:Birds:647791</t>
-  </si>
-  <si>
-    <t>647791</t>
-  </si>
-  <si>
-    <t>F04</t>
+    <t>USNM:Birds:647792</t>
+  </si>
+  <si>
+    <t>647792</t>
+  </si>
+  <si>
+    <t>Hippolais pallida</t>
+  </si>
+  <si>
+    <t>Sylviidae</t>
+  </si>
+  <si>
+    <t>Hippolais</t>
+  </si>
+  <si>
+    <t>pallida</t>
+  </si>
+  <si>
+    <t>G04</t>
   </si>
   <si>
     <t>AmD_Tissue_31</t>
   </si>
   <si>
-    <t>USNM:Birds:647792</t>
-  </si>
-  <si>
-    <t>647792</t>
-  </si>
-  <si>
-    <t>Hippolais pallida</t>
-  </si>
-  <si>
-    <t>Sylviidae</t>
-  </si>
-  <si>
-    <t>Hippolais</t>
-  </si>
-  <si>
-    <t>pallida</t>
-  </si>
-  <si>
-    <t>G04</t>
+    <t>USNM:Birds:647793</t>
+  </si>
+  <si>
+    <t>647793</t>
+  </si>
+  <si>
+    <t>Riparia riparia</t>
+  </si>
+  <si>
+    <t>Riparia</t>
+  </si>
+  <si>
+    <t>riparia</t>
+  </si>
+  <si>
+    <t>H04</t>
   </si>
   <si>
     <t>AmD_Tissue_32</t>
   </si>
   <si>
-    <t>USNM:Birds:647793</t>
-  </si>
-  <si>
-    <t>647793</t>
-  </si>
-  <si>
-    <t>Riparia riparia</t>
-  </si>
-  <si>
-    <t>Riparia</t>
-  </si>
-  <si>
-    <t>riparia</t>
-  </si>
-  <si>
-    <t>H04</t>
+    <t>USNM:Birds:647794</t>
+  </si>
+  <si>
+    <t>647794</t>
+  </si>
+  <si>
+    <t>Merops albicollis</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>albicollis</t>
+  </si>
+  <si>
+    <t>A05</t>
   </si>
   <si>
     <t>AmD_Tissue_33</t>
   </si>
   <si>
-    <t>USNM:Birds:647794</t>
-  </si>
-  <si>
-    <t>647794</t>
-  </si>
-  <si>
-    <t>Merops albicollis</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>albicollis</t>
-  </si>
-  <si>
-    <t>A05</t>
+    <t>USNM:Birds:647795</t>
+  </si>
+  <si>
+    <t>647795</t>
+  </si>
+  <si>
+    <t>B05</t>
   </si>
   <si>
     <t>AmD_Tissue_34</t>
   </si>
   <si>
-    <t>USNM:Birds:647795</t>
-  </si>
-  <si>
-    <t>647795</t>
-  </si>
-  <si>
-    <t>B05</t>
+    <t>USNM:Birds:647796</t>
+  </si>
+  <si>
+    <t>647796</t>
+  </si>
+  <si>
+    <t>M. Spradley</t>
+  </si>
+  <si>
+    <t>C05</t>
   </si>
   <si>
     <t>AmD_Tissue_35</t>
   </si>
   <si>
-    <t>USNM:Birds:647796</t>
-  </si>
-  <si>
-    <t>647796</t>
-  </si>
-  <si>
-    <t>M. Spradley</t>
-  </si>
-  <si>
-    <t>C05</t>
+    <t>USNM:Birds:647797</t>
+  </si>
+  <si>
+    <t>647797</t>
+  </si>
+  <si>
+    <t>Anthreptes platurus</t>
+  </si>
+  <si>
+    <t>Anthreptes</t>
+  </si>
+  <si>
+    <t>platurus</t>
+  </si>
+  <si>
+    <t>D05</t>
   </si>
   <si>
     <t>AmD_Tissue_36</t>
   </si>
   <si>
-    <t>USNM:Birds:647797</t>
-  </si>
-  <si>
-    <t>647797</t>
-  </si>
-  <si>
-    <t>Anthreptes platurus</t>
-  </si>
-  <si>
-    <t>Anthreptes</t>
-  </si>
-  <si>
-    <t>platurus</t>
-  </si>
-  <si>
-    <t>D05</t>
+    <t>USNM:Birds:647798</t>
+  </si>
+  <si>
+    <t>647798</t>
+  </si>
+  <si>
+    <t>E05</t>
   </si>
   <si>
     <t>AmD_Tissue_37</t>
   </si>
   <si>
-    <t>USNM:Birds:647798</t>
-  </si>
-  <si>
-    <t>647798</t>
-  </si>
-  <si>
-    <t>E05</t>
+    <t>USNM:Birds:647893</t>
+  </si>
+  <si>
+    <t>647893</t>
+  </si>
+  <si>
+    <t>Columba livia</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Columba</t>
+  </si>
+  <si>
+    <t>livia</t>
+  </si>
+  <si>
+    <t>F05</t>
   </si>
   <si>
     <t>AmD_Tissue_38</t>
   </si>
   <si>
-    <t>USNM:Birds:647893</t>
-  </si>
-  <si>
-    <t>647893</t>
-  </si>
-  <si>
-    <t>Columba livia</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Columba</t>
-  </si>
-  <si>
-    <t>livia</t>
-  </si>
-  <si>
-    <t>F05</t>
+    <t>USNM:Birds:647800</t>
+  </si>
+  <si>
+    <t>647800</t>
+  </si>
+  <si>
+    <t>G05</t>
   </si>
   <si>
     <t>AmD_Tissue_39</t>
   </si>
   <si>
-    <t>USNM:Birds:647800</t>
-  </si>
-  <si>
-    <t>647800</t>
-  </si>
-  <si>
-    <t>G05</t>
+    <t>USNM:Birds:647801</t>
+  </si>
+  <si>
+    <t>647801</t>
+  </si>
+  <si>
+    <t>H05</t>
   </si>
   <si>
     <t>AmD_Tissue_40</t>
   </si>
   <si>
-    <t>USNM:Birds:647801</t>
-  </si>
-  <si>
-    <t>647801</t>
-  </si>
-  <si>
-    <t>H05</t>
+    <t>USNM:Birds:647802</t>
+  </si>
+  <si>
+    <t>647802</t>
+  </si>
+  <si>
+    <t>Apus affinis</t>
+  </si>
+  <si>
+    <t>Chabelley Airfield, ca 6 km SW Balbala</t>
+  </si>
+  <si>
+    <t>11.5167</t>
+  </si>
+  <si>
+    <t>43.0667</t>
+  </si>
+  <si>
+    <t>Apodiformes</t>
+  </si>
+  <si>
+    <t>Apodidae</t>
+  </si>
+  <si>
+    <t>Apus</t>
+  </si>
+  <si>
+    <t>affinis</t>
+  </si>
+  <si>
+    <t>A06</t>
   </si>
   <si>
     <t>AmD_Tissue_41</t>
   </si>
   <si>
-    <t>USNM:Birds:647802</t>
-  </si>
-  <si>
-    <t>647802</t>
-  </si>
-  <si>
-    <t>Apus affinis</t>
-  </si>
-  <si>
-    <t>Chabelley Airfield, ca 6 km SW Balbala</t>
-  </si>
-  <si>
-    <t>11.5167</t>
-  </si>
-  <si>
-    <t>43.0667</t>
-  </si>
-  <si>
-    <t>Apodiformes</t>
-  </si>
-  <si>
-    <t>Apodidae</t>
-  </si>
-  <si>
-    <t>Apus</t>
-  </si>
-  <si>
-    <t>affinis</t>
-  </si>
-  <si>
-    <t>A06</t>
+    <t>USNM:Birds:647803</t>
+  </si>
+  <si>
+    <t>647803</t>
+  </si>
+  <si>
+    <t>Trachyphonus margaritatus</t>
+  </si>
+  <si>
+    <t>Piciformes</t>
+  </si>
+  <si>
+    <t>Capitonidae</t>
+  </si>
+  <si>
+    <t>Trachyphonus</t>
+  </si>
+  <si>
+    <t>margaritatus</t>
+  </si>
+  <si>
+    <t>B06</t>
   </si>
   <si>
     <t>AmD_Tissue_42</t>
   </si>
   <si>
-    <t>USNM:Birds:647803</t>
-  </si>
-  <si>
-    <t>647803</t>
-  </si>
-  <si>
-    <t>Trachyphonus margaritatus</t>
-  </si>
-  <si>
-    <t>Piciformes</t>
-  </si>
-  <si>
-    <t>Capitonidae</t>
-  </si>
-  <si>
-    <t>Trachyphonus</t>
-  </si>
-  <si>
-    <t>margaritatus</t>
-  </si>
-  <si>
-    <t>B06</t>
+    <t>USNM:Birds:647910</t>
+  </si>
+  <si>
+    <t>647910</t>
+  </si>
+  <si>
+    <t>Bubulcus ibis</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Bubulcus</t>
+  </si>
+  <si>
+    <t>ibis</t>
+  </si>
+  <si>
+    <t>C06</t>
   </si>
   <si>
     <t>AmD_Tissue_43</t>
   </si>
   <si>
-    <t>USNM:Birds:647910</t>
-  </si>
-  <si>
-    <t>647910</t>
-  </si>
-  <si>
-    <t>Bubulcus ibis</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>Bubulcus</t>
-  </si>
-  <si>
-    <t>ibis</t>
-  </si>
-  <si>
-    <t>C06</t>
+    <t>USNM:Birds:647804</t>
+  </si>
+  <si>
+    <t>647804</t>
+  </si>
+  <si>
+    <t>Nectarinia habessinica</t>
+  </si>
+  <si>
+    <t>M. Desrosiers</t>
+  </si>
+  <si>
+    <t>habessinica</t>
+  </si>
+  <si>
+    <t>D06</t>
   </si>
   <si>
     <t>AmD_Tissue_44</t>
   </si>
   <si>
-    <t>USNM:Birds:647804</t>
-  </si>
-  <si>
-    <t>647804</t>
-  </si>
-  <si>
-    <t>Nectarinia habessinica</t>
-  </si>
-  <si>
-    <t>M. Desrosiers</t>
-  </si>
-  <si>
-    <t>habessinica</t>
-  </si>
-  <si>
-    <t>D06</t>
+    <t>USNM:Birds:647805</t>
+  </si>
+  <si>
+    <t>647805</t>
+  </si>
+  <si>
+    <t>E06</t>
   </si>
   <si>
     <t>AmD_Tissue_45</t>
   </si>
   <si>
-    <t>USNM:Birds:647805</t>
-  </si>
-  <si>
-    <t>647805</t>
-  </si>
-  <si>
-    <t>E06</t>
+    <t>USNM:Birds:647806</t>
+  </si>
+  <si>
+    <t>647806</t>
+  </si>
+  <si>
+    <t>Phylloscopus trochilus</t>
+  </si>
+  <si>
+    <t>B. McGuinness</t>
+  </si>
+  <si>
+    <t>Phylloscopus</t>
+  </si>
+  <si>
+    <t>trochilus</t>
+  </si>
+  <si>
+    <t>F06</t>
   </si>
   <si>
     <t>AmD_Tissue_46</t>
   </si>
   <si>
-    <t>USNM:Birds:647806</t>
-  </si>
-  <si>
-    <t>647806</t>
-  </si>
-  <si>
-    <t>Phylloscopus trochilus</t>
-  </si>
-  <si>
-    <t>B. McGuinness</t>
-  </si>
-  <si>
-    <t>Phylloscopus</t>
-  </si>
-  <si>
-    <t>trochilus</t>
-  </si>
-  <si>
-    <t>F06</t>
+    <t>USNM:Birds:647807</t>
+  </si>
+  <si>
+    <t>647807</t>
+  </si>
+  <si>
+    <t>G06</t>
   </si>
   <si>
     <t>AmD_Tissue_47</t>
   </si>
   <si>
-    <t>USNM:Birds:647807</t>
-  </si>
-  <si>
-    <t>647807</t>
-  </si>
-  <si>
-    <t>G06</t>
+    <t>USNM:Birds:647808</t>
+  </si>
+  <si>
+    <t>647808</t>
+  </si>
+  <si>
+    <t>H06</t>
   </si>
   <si>
     <t>AmD_Tissue_48</t>
   </si>
   <si>
-    <t>USNM:Birds:647808</t>
-  </si>
-  <si>
-    <t>647808</t>
-  </si>
-  <si>
-    <t>H06</t>
+    <t>USNM:Birds:647809</t>
+  </si>
+  <si>
+    <t>647809</t>
+  </si>
+  <si>
+    <t>Cercomela melanura</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Cercomela</t>
+  </si>
+  <si>
+    <t>melanura</t>
+  </si>
+  <si>
+    <t>A07</t>
   </si>
   <si>
     <t>AmD_Tissue_49</t>
   </si>
   <si>
-    <t>USNM:Birds:647809</t>
-  </si>
-  <si>
-    <t>647809</t>
-  </si>
-  <si>
-    <t>Cercomela melanura</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Cercomela</t>
-  </si>
-  <si>
-    <t>melanura</t>
-  </si>
-  <si>
-    <t>A07</t>
+    <t>USNM:Birds:647810</t>
+  </si>
+  <si>
+    <t>647810</t>
+  </si>
+  <si>
+    <t>B07</t>
   </si>
   <si>
     <t>AmD_Tissue_50</t>
   </si>
   <si>
-    <t>USNM:Birds:647810</t>
-  </si>
-  <si>
-    <t>647810</t>
-  </si>
-  <si>
-    <t>B07</t>
+    <t>USNM:Birds:647763</t>
+  </si>
+  <si>
+    <t>647763</t>
+  </si>
+  <si>
+    <t>M. Zaragosa</t>
+  </si>
+  <si>
+    <t>C07</t>
   </si>
   <si>
     <t>AmD_Tissue_51</t>
   </si>
   <si>
-    <t>USNM:Birds:647763</t>
-  </si>
-  <si>
-    <t>647763</t>
-  </si>
-  <si>
-    <t>M. Zaragosa</t>
-  </si>
-  <si>
-    <t>C07</t>
+    <t>USNM:Birds:647812</t>
+  </si>
+  <si>
+    <t>647812</t>
+  </si>
+  <si>
+    <t>D07</t>
   </si>
   <si>
     <t>AmD_Tissue_52</t>
   </si>
   <si>
-    <t>USNM:Birds:647812</t>
-  </si>
-  <si>
-    <t>647812</t>
-  </si>
-  <si>
-    <t>D07</t>
+    <t>USNM:Birds:647813</t>
+  </si>
+  <si>
+    <t>647813</t>
+  </si>
+  <si>
+    <t>Ciconia abdimii</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>B. Ronnau</t>
+  </si>
+  <si>
+    <t>Ciconiidae</t>
+  </si>
+  <si>
+    <t>Ciconia</t>
+  </si>
+  <si>
+    <t>abdimii</t>
+  </si>
+  <si>
+    <t>E07</t>
   </si>
   <si>
     <t>AmD_Tissue_53</t>
   </si>
   <si>
-    <t>USNM:Birds:647813</t>
-  </si>
-  <si>
-    <t>647813</t>
-  </si>
-  <si>
-    <t>Ciconia abdimii</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>B. Ronnau</t>
-  </si>
-  <si>
-    <t>Ciconiidae</t>
-  </si>
-  <si>
-    <t>Ciconia</t>
-  </si>
-  <si>
-    <t>abdimii</t>
-  </si>
-  <si>
-    <t>E07</t>
+    <t>USNM:Birds:647815</t>
+  </si>
+  <si>
+    <t>647815</t>
+  </si>
+  <si>
+    <t>Numenius phaeopus</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Numenius</t>
+  </si>
+  <si>
+    <t>phaeopus</t>
+  </si>
+  <si>
+    <t>F07</t>
   </si>
   <si>
     <t>AmD_Tissue_54</t>
   </si>
   <si>
-    <t>USNM:Birds:647815</t>
-  </si>
-  <si>
-    <t>647815</t>
-  </si>
-  <si>
-    <t>Numenius phaeopus</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Numenius</t>
-  </si>
-  <si>
-    <t>phaeopus</t>
-  </si>
-  <si>
-    <t>F07</t>
+    <t>USNM:Birds:647816</t>
+  </si>
+  <si>
+    <t>647816</t>
+  </si>
+  <si>
+    <t>Charadrius hiaticula</t>
+  </si>
+  <si>
+    <t>Charadriidae</t>
+  </si>
+  <si>
+    <t>Charadrius</t>
+  </si>
+  <si>
+    <t>hiaticula</t>
+  </si>
+  <si>
+    <t>G07</t>
   </si>
   <si>
     <t>AmD_Tissue_55</t>
   </si>
   <si>
-    <t>USNM:Birds:647816</t>
-  </si>
-  <si>
-    <t>647816</t>
-  </si>
-  <si>
-    <t>Charadrius hiaticula</t>
-  </si>
-  <si>
-    <t>Charadriidae</t>
-  </si>
-  <si>
-    <t>Charadrius</t>
-  </si>
-  <si>
-    <t>hiaticula</t>
-  </si>
-  <si>
-    <t>G07</t>
+    <t>USNM:Birds:647817</t>
+  </si>
+  <si>
+    <t>647817</t>
+  </si>
+  <si>
+    <t>Larus hemprichii</t>
+  </si>
+  <si>
+    <t>Laridae</t>
+  </si>
+  <si>
+    <t>Larus</t>
+  </si>
+  <si>
+    <t>hemprichii</t>
+  </si>
+  <si>
+    <t>H07</t>
   </si>
   <si>
     <t>AmD_Tissue_56</t>
   </si>
   <si>
-    <t>USNM:Birds:647817</t>
-  </si>
-  <si>
-    <t>647817</t>
-  </si>
-  <si>
-    <t>Larus hemprichii</t>
-  </si>
-  <si>
-    <t>Laridae</t>
-  </si>
-  <si>
-    <t>Larus</t>
-  </si>
-  <si>
-    <t>hemprichii</t>
-  </si>
-  <si>
-    <t>H07</t>
+    <t>USNM:Birds:647818</t>
+  </si>
+  <si>
+    <t>647818</t>
+  </si>
+  <si>
+    <t>Pterocles lichtensteinii</t>
+  </si>
+  <si>
+    <t>Ambouli River, ca 5.5 km SW Balbala</t>
+  </si>
+  <si>
+    <t>11.5194</t>
+  </si>
+  <si>
+    <t>43.0986</t>
+  </si>
+  <si>
+    <t>J. Winjum</t>
+  </si>
+  <si>
+    <t>Pteroclididae</t>
+  </si>
+  <si>
+    <t>Pterocles</t>
+  </si>
+  <si>
+    <t>lichtensteinii</t>
+  </si>
+  <si>
+    <t>A08</t>
   </si>
   <si>
     <t>AmD_Tissue_57</t>
   </si>
   <si>
-    <t>USNM:Birds:647818</t>
-  </si>
-  <si>
-    <t>647818</t>
-  </si>
-  <si>
-    <t>Pterocles lichtensteinii</t>
-  </si>
-  <si>
-    <t>Ambouli River, ca 5.5 km SW Balbala</t>
-  </si>
-  <si>
-    <t>11.5194</t>
-  </si>
-  <si>
-    <t>43.0986</t>
-  </si>
-  <si>
-    <t>J. Winjum</t>
-  </si>
-  <si>
-    <t>Pteroclididae</t>
-  </si>
-  <si>
-    <t>Pterocles</t>
-  </si>
-  <si>
-    <t>lichtensteinii</t>
-  </si>
-  <si>
-    <t>A08</t>
+    <t>USNM:Birds:647879</t>
+  </si>
+  <si>
+    <t>647879</t>
+  </si>
+  <si>
+    <t>B08</t>
   </si>
   <si>
     <t>AmD_Tissue_58</t>
   </si>
   <si>
-    <t>USNM:Birds:647879</t>
-  </si>
-  <si>
-    <t>647879</t>
-  </si>
-  <si>
-    <t>B08</t>
+    <t>USNM:Birds:647819</t>
+  </si>
+  <si>
+    <t>647819</t>
+  </si>
+  <si>
+    <t>Estrilda rhodopyga</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Estrilda</t>
+  </si>
+  <si>
+    <t>rhodopyga</t>
+  </si>
+  <si>
+    <t>C08</t>
   </si>
   <si>
     <t>AmD_Tissue_59</t>
   </si>
   <si>
-    <t>USNM:Birds:647819</t>
-  </si>
-  <si>
-    <t>647819</t>
-  </si>
-  <si>
-    <t>Estrilda rhodopyga</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Estrilda</t>
-  </si>
-  <si>
-    <t>rhodopyga</t>
-  </si>
-  <si>
-    <t>C08</t>
+    <t>USNM:Birds:647820</t>
+  </si>
+  <si>
+    <t>647820</t>
+  </si>
+  <si>
+    <t>Charadrius alexandrinus</t>
+  </si>
+  <si>
+    <t>alexandrinus</t>
+  </si>
+  <si>
+    <t>D08</t>
   </si>
   <si>
     <t>AmD_Tissue_60</t>
   </si>
   <si>
-    <t>USNM:Birds:647820</t>
-  </si>
-  <si>
-    <t>647820</t>
-  </si>
-  <si>
-    <t>Charadrius alexandrinus</t>
-  </si>
-  <si>
-    <t>alexandrinus</t>
-  </si>
-  <si>
-    <t>D08</t>
+    <t>USNM:Birds:647822</t>
+  </si>
+  <si>
+    <t>647822</t>
+  </si>
+  <si>
+    <t>Locustella fluviatilis</t>
+  </si>
+  <si>
+    <t>Locustella</t>
+  </si>
+  <si>
+    <t>fluviatilis</t>
+  </si>
+  <si>
+    <t>E08</t>
   </si>
   <si>
     <t>AmD_Tissue_61</t>
   </si>
   <si>
-    <t>USNM:Birds:647822</t>
-  </si>
-  <si>
-    <t>647822</t>
-  </si>
-  <si>
-    <t>Locustella fluviatilis</t>
-  </si>
-  <si>
-    <t>Locustella</t>
-  </si>
-  <si>
-    <t>fluviatilis</t>
-  </si>
-  <si>
-    <t>E08</t>
+    <t>USNM:Birds:647823</t>
+  </si>
+  <si>
+    <t>647823</t>
+  </si>
+  <si>
+    <t>F08</t>
   </si>
   <si>
     <t>AmD_Tissue_62</t>
   </si>
   <si>
-    <t>USNM:Birds:647823</t>
-  </si>
-  <si>
-    <t>647823</t>
-  </si>
-  <si>
-    <t>F08</t>
+    <t>USNM:Birds:647824</t>
+  </si>
+  <si>
+    <t>647824</t>
+  </si>
+  <si>
+    <t>G08</t>
   </si>
   <si>
     <t>AmD_Tissue_63</t>
   </si>
   <si>
-    <t>USNM:Birds:647824</t>
-  </si>
-  <si>
-    <t>647824</t>
-  </si>
-  <si>
-    <t>G08</t>
+    <t>USNM:Birds:647825</t>
+  </si>
+  <si>
+    <t>647825</t>
+  </si>
+  <si>
+    <t>Eremopterix nigriceps</t>
+  </si>
+  <si>
+    <t>Alaudidae</t>
+  </si>
+  <si>
+    <t>Eremopterix</t>
+  </si>
+  <si>
+    <t>nigriceps</t>
+  </si>
+  <si>
+    <t>H08</t>
   </si>
   <si>
     <t>AmD_Tissue_64</t>
   </si>
   <si>
-    <t>USNM:Birds:647825</t>
-  </si>
-  <si>
-    <t>647825</t>
-  </si>
-  <si>
-    <t>Eremopterix nigriceps</t>
-  </si>
-  <si>
-    <t>Alaudidae</t>
-  </si>
-  <si>
-    <t>Eremopterix</t>
-  </si>
-  <si>
-    <t>nigriceps</t>
-  </si>
-  <si>
-    <t>H08</t>
+    <t>USNM:Birds:647826</t>
+  </si>
+  <si>
+    <t>647826</t>
+  </si>
+  <si>
+    <t>A09</t>
   </si>
   <si>
     <t>AmD_Tissue_65</t>
   </si>
   <si>
-    <t>USNM:Birds:647826</t>
-  </si>
-  <si>
-    <t>647826</t>
-  </si>
-  <si>
-    <t>A09</t>
+    <t>USNM:Birds:647827</t>
+  </si>
+  <si>
+    <t>647827</t>
+  </si>
+  <si>
+    <t>Prinia gracilis</t>
+  </si>
+  <si>
+    <t>A. Peterson</t>
+  </si>
+  <si>
+    <t>Prinia</t>
+  </si>
+  <si>
+    <t>gracilis</t>
+  </si>
+  <si>
+    <t>B09</t>
   </si>
   <si>
     <t>AmD_Tissue_66</t>
   </si>
   <si>
-    <t>USNM:Birds:647827</t>
-  </si>
-  <si>
-    <t>647827</t>
-  </si>
-  <si>
-    <t>Prinia gracilis</t>
-  </si>
-  <si>
-    <t>A. Peterson</t>
-  </si>
-  <si>
-    <t>Prinia</t>
-  </si>
-  <si>
-    <t>gracilis</t>
-  </si>
-  <si>
-    <t>B09</t>
+    <t>USNM:Birds:647828</t>
+  </si>
+  <si>
+    <t>647828</t>
+  </si>
+  <si>
+    <t>C09</t>
   </si>
   <si>
     <t>AmD_Tissue_67</t>
   </si>
   <si>
-    <t>USNM:Birds:647828</t>
-  </si>
-  <si>
-    <t>647828</t>
-  </si>
-  <si>
-    <t>C09</t>
+    <t>USNM:Birds:647829</t>
+  </si>
+  <si>
+    <t>647829</t>
+  </si>
+  <si>
+    <t>D09</t>
   </si>
   <si>
     <t>AmD_Tissue_68</t>
   </si>
   <si>
-    <t>USNM:Birds:647829</t>
-  </si>
-  <si>
-    <t>647829</t>
-  </si>
-  <si>
-    <t>D09</t>
+    <t>USNM:Birds:647894</t>
+  </si>
+  <si>
+    <t>647894</t>
+  </si>
+  <si>
+    <t>R. Nelson</t>
+  </si>
+  <si>
+    <t>E09</t>
   </si>
   <si>
     <t>AmD_Tissue_69</t>
   </si>
   <si>
-    <t>USNM:Birds:647894</t>
-  </si>
-  <si>
-    <t>647894</t>
-  </si>
-  <si>
-    <t>R. Nelson</t>
-  </si>
-  <si>
-    <t>E09</t>
+    <t>USNM:Birds:647831</t>
+  </si>
+  <si>
+    <t>647831</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>F09</t>
   </si>
   <si>
     <t>AmD_Tissue_70</t>
   </si>
   <si>
-    <t>USNM:Birds:647831</t>
-  </si>
-  <si>
-    <t>647831</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>F09</t>
+    <t>USNM:Birds:647832</t>
+  </si>
+  <si>
+    <t>647832</t>
+  </si>
+  <si>
+    <t>G09</t>
   </si>
   <si>
     <t>AmD_Tissue_71</t>
   </si>
   <si>
-    <t>USNM:Birds:647832</t>
-  </si>
-  <si>
-    <t>647832</t>
-  </si>
-  <si>
-    <t>G09</t>
+    <t>USNM:Birds:647833</t>
+  </si>
+  <si>
+    <t>647833</t>
+  </si>
+  <si>
+    <t>H09</t>
   </si>
   <si>
     <t>AmD_Tissue_72</t>
   </si>
   <si>
-    <t>USNM:Birds:647833</t>
-  </si>
-  <si>
-    <t>647833</t>
-  </si>
-  <si>
-    <t>H09</t>
+    <t>USNM:Birds:647834</t>
+  </si>
+  <si>
+    <t>647834</t>
+  </si>
+  <si>
+    <t>A10</t>
   </si>
   <si>
     <t>AmD_Tissue_73</t>
   </si>
   <si>
-    <t>USNM:Birds:647834</t>
-  </si>
-  <si>
-    <t>647834</t>
-  </si>
-  <si>
-    <t>A10</t>
+    <t>USNM:Birds:647835</t>
+  </si>
+  <si>
+    <t>647835</t>
+  </si>
+  <si>
+    <t>B10</t>
   </si>
   <si>
     <t>AmD_Tissue_74</t>
   </si>
   <si>
-    <t>USNM:Birds:647835</t>
-  </si>
-  <si>
-    <t>647835</t>
-  </si>
-  <si>
-    <t>B10</t>
+    <t>USNM:Birds:647836</t>
+  </si>
+  <si>
+    <t>647836</t>
+  </si>
+  <si>
+    <t>Sterna nilotica</t>
+  </si>
+  <si>
+    <t>Sterna</t>
+  </si>
+  <si>
+    <t>nilotica</t>
+  </si>
+  <si>
+    <t>C10</t>
   </si>
   <si>
     <t>AmD_Tissue_75</t>
   </si>
   <si>
-    <t>USNM:Birds:647836</t>
-  </si>
-  <si>
-    <t>647836</t>
-  </si>
-  <si>
-    <t>Sterna nilotica</t>
-  </si>
-  <si>
-    <t>Sterna</t>
-  </si>
-  <si>
-    <t>nilotica</t>
-  </si>
-  <si>
-    <t>C10</t>
+    <t>USNM:Birds:647837</t>
+  </si>
+  <si>
+    <t>647837</t>
+  </si>
+  <si>
+    <t>D10</t>
   </si>
   <si>
     <t>AmD_Tissue_76</t>
   </si>
   <si>
-    <t>USNM:Birds:647837</t>
-  </si>
-  <si>
-    <t>647837</t>
-  </si>
-  <si>
-    <t>D10</t>
+    <t>USNM:Birds:647838</t>
+  </si>
+  <si>
+    <t>647838</t>
+  </si>
+  <si>
+    <t>Columba guinea</t>
+  </si>
+  <si>
+    <t>guinea</t>
+  </si>
+  <si>
+    <t>E10</t>
   </si>
   <si>
     <t>AmD_Tissue_77</t>
   </si>
   <si>
-    <t>USNM:Birds:647838</t>
-  </si>
-  <si>
-    <t>647838</t>
-  </si>
-  <si>
-    <t>Columba guinea</t>
-  </si>
-  <si>
-    <t>guinea</t>
-  </si>
-  <si>
-    <t>E10</t>
+    <t>USNM:Birds:647839</t>
+  </si>
+  <si>
+    <t>647839</t>
+  </si>
+  <si>
+    <t>Acrocephalus scirpaceus</t>
+  </si>
+  <si>
+    <t>Acrocephalus</t>
+  </si>
+  <si>
+    <t>scirpaceus</t>
+  </si>
+  <si>
+    <t>F10</t>
   </si>
   <si>
     <t>AmD_Tissue_78</t>
   </si>
   <si>
-    <t>USNM:Birds:647839</t>
-  </si>
-  <si>
-    <t>647839</t>
-  </si>
-  <si>
-    <t>Acrocephalus scirpaceus</t>
-  </si>
-  <si>
-    <t>Acrocephalus</t>
-  </si>
-  <si>
-    <t>scirpaceus</t>
-  </si>
-  <si>
-    <t>F10</t>
+    <t>USNM:Birds:647895</t>
+  </si>
+  <si>
+    <t>647895</t>
+  </si>
+  <si>
+    <t>Arenaria interpres</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Arenaria</t>
+  </si>
+  <si>
+    <t>interpres</t>
+  </si>
+  <si>
+    <t>G10</t>
   </si>
   <si>
     <t>AmD_Tissue_79</t>
   </si>
   <si>
-    <t>USNM:Birds:647895</t>
-  </si>
-  <si>
-    <t>647895</t>
-  </si>
-  <si>
-    <t>Arenaria interpres</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>Arenaria</t>
-  </si>
-  <si>
-    <t>interpres</t>
-  </si>
-  <si>
-    <t>G10</t>
+    <t>USNM:Birds:647911</t>
+  </si>
+  <si>
+    <t>647911</t>
+  </si>
+  <si>
+    <t>H10</t>
   </si>
   <si>
     <t>AmD_Tissue_80</t>
   </si>
   <si>
-    <t>USNM:Birds:647911</t>
-  </si>
-  <si>
-    <t>647911</t>
-  </si>
-  <si>
-    <t>H10</t>
+    <t>USNM:Birds:647896</t>
+  </si>
+  <si>
+    <t>647896</t>
+  </si>
+  <si>
+    <t>A11</t>
   </si>
   <si>
     <t>AmD_Tissue_81</t>
   </si>
   <si>
-    <t>USNM:Birds:647896</t>
-  </si>
-  <si>
-    <t>647896</t>
-  </si>
-  <si>
-    <t>A11</t>
+    <t>USNM:Birds:647912</t>
+  </si>
+  <si>
+    <t>647912</t>
+  </si>
+  <si>
+    <t>Vanellus spinosus</t>
+  </si>
+  <si>
+    <t>Vanellus</t>
+  </si>
+  <si>
+    <t>spinosus</t>
+  </si>
+  <si>
+    <t>B11</t>
   </si>
   <si>
     <t>AmD_Tissue_82</t>
   </si>
   <si>
-    <t>USNM:Birds:647912</t>
-  </si>
-  <si>
-    <t>647912</t>
-  </si>
-  <si>
-    <t>Vanellus spinosus</t>
-  </si>
-  <si>
-    <t>Vanellus</t>
-  </si>
-  <si>
-    <t>spinosus</t>
-  </si>
-  <si>
-    <t>B11</t>
+    <t>USNM:Birds:647897</t>
+  </si>
+  <si>
+    <t>647897</t>
+  </si>
+  <si>
+    <t>C11</t>
   </si>
   <si>
     <t>AmD_Tissue_83</t>
   </si>
   <si>
-    <t>USNM:Birds:647897</t>
-  </si>
-  <si>
-    <t>647897</t>
-  </si>
-  <si>
-    <t>C11</t>
+    <t>USNM:Birds:647913</t>
+  </si>
+  <si>
+    <t>647913</t>
+  </si>
+  <si>
+    <t>D11</t>
   </si>
   <si>
     <t>AmD_Tissue_84</t>
   </si>
   <si>
-    <t>USNM:Birds:647913</t>
-  </si>
-  <si>
-    <t>647913</t>
-  </si>
-  <si>
-    <t>D11</t>
+    <t>USNM:Birds:647914</t>
+  </si>
+  <si>
+    <t>647914</t>
+  </si>
+  <si>
+    <t>E11</t>
   </si>
   <si>
     <t>AmD_Tissue_85</t>
   </si>
   <si>
-    <t>USNM:Birds:647914</t>
-  </si>
-  <si>
-    <t>647914</t>
-  </si>
-  <si>
-    <t>E11</t>
+    <t>USNM:Birds:647840</t>
+  </si>
+  <si>
+    <t>647840</t>
+  </si>
+  <si>
+    <t>Larus fuscus</t>
+  </si>
+  <si>
+    <t>fuscus</t>
+  </si>
+  <si>
+    <t>F11</t>
   </si>
   <si>
     <t>AmD_Tissue_86</t>
   </si>
   <si>
-    <t>USNM:Birds:647840</t>
-  </si>
-  <si>
-    <t>647840</t>
-  </si>
-  <si>
-    <t>Larus fuscus</t>
-  </si>
-  <si>
-    <t>fuscus</t>
-  </si>
-  <si>
-    <t>F11</t>
+    <t>USNM:Birds:647916</t>
+  </si>
+  <si>
+    <t>647916</t>
+  </si>
+  <si>
+    <t>G11</t>
   </si>
   <si>
     <t>AmD_Tissue_87</t>
   </si>
   <si>
-    <t>USNM:Birds:647916</t>
-  </si>
-  <si>
-    <t>647916</t>
-  </si>
-  <si>
-    <t>G11</t>
+    <t>USNM:Birds:647917</t>
+  </si>
+  <si>
+    <t>647917</t>
+  </si>
+  <si>
+    <t>H11</t>
   </si>
   <si>
     <t>AmD_Tissue_88</t>
   </si>
   <si>
-    <t>USNM:Birds:647917</t>
-  </si>
-  <si>
-    <t>647917</t>
-  </si>
-  <si>
-    <t>H11</t>
+    <t>USNM:Birds:647918</t>
+  </si>
+  <si>
+    <t>647918</t>
+  </si>
+  <si>
+    <t>A12</t>
   </si>
   <si>
     <t>AmD_Tissue_89</t>
   </si>
   <si>
-    <t>USNM:Birds:647918</t>
-  </si>
-  <si>
-    <t>647918</t>
-  </si>
-  <si>
-    <t>A12</t>
+    <t>USNM:Birds:647919</t>
+  </si>
+  <si>
+    <t>647919</t>
+  </si>
+  <si>
+    <t>Sterna anaethetus</t>
+  </si>
+  <si>
+    <t>anaethetus</t>
+  </si>
+  <si>
+    <t>B12</t>
   </si>
   <si>
     <t>AmD_Tissue_90</t>
   </si>
   <si>
-    <t>USNM:Birds:647919</t>
-  </si>
-  <si>
-    <t>647919</t>
-  </si>
-  <si>
-    <t>Sterna anaethetus</t>
-  </si>
-  <si>
-    <t>anaethetus</t>
-  </si>
-  <si>
-    <t>B12</t>
+    <t>USNM:Birds:647841</t>
+  </si>
+  <si>
+    <t>647841</t>
+  </si>
+  <si>
+    <t>Pluvialis squatarola</t>
+  </si>
+  <si>
+    <t>Pluvialis</t>
+  </si>
+  <si>
+    <t>squatarola</t>
+  </si>
+  <si>
+    <t>C12</t>
   </si>
   <si>
     <t>AmD_Tissue_91</t>
   </si>
   <si>
-    <t>USNM:Birds:647841</t>
-  </si>
-  <si>
-    <t>647841</t>
-  </si>
-  <si>
-    <t>Pluvialis squatarola</t>
-  </si>
-  <si>
-    <t>Pluvialis</t>
-  </si>
-  <si>
-    <t>squatarola</t>
-  </si>
-  <si>
-    <t>C12</t>
+    <t>USNM:Birds:647921</t>
+  </si>
+  <si>
+    <t>647921</t>
+  </si>
+  <si>
+    <t>D12</t>
   </si>
   <si>
     <t>AmD_Tissue_92</t>
   </si>
   <si>
-    <t>USNM:Birds:647921</t>
-  </si>
-  <si>
-    <t>647921</t>
-  </si>
-  <si>
-    <t>D12</t>
+    <t>USNM:Birds:647922</t>
+  </si>
+  <si>
+    <t>647922</t>
+  </si>
+  <si>
+    <t>E12</t>
   </si>
   <si>
     <t>AmD_Tissue_93</t>
   </si>
   <si>
-    <t>USNM:Birds:647922</t>
-  </si>
-  <si>
-    <t>647922</t>
-  </si>
-  <si>
-    <t>E12</t>
+    <t>USNM:Birds:647923</t>
+  </si>
+  <si>
+    <t>647923</t>
+  </si>
+  <si>
+    <t>F12</t>
   </si>
   <si>
     <t>AmD_Tissue_94</t>
-  </si>
-  <si>
-    <t>USNM:Birds:647923</t>
-  </si>
-  <si>
-    <t>647923</t>
-  </si>
-  <si>
-    <t>F12</t>
-  </si>
-  <si>
-    <t>AmD_Tissue_95</t>
   </si>
   <si>
     <t>USNM:Birds:647924</t>

</xml_diff>